<commit_message>
Changed repo name to Planning
</commit_message>
<xml_diff>
--- a/Goals.xlsx
+++ b/Goals.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://toolupcom-my.sharepoint.com/personal/solomon_manamel_pcstools_com/Documents/Desktop/Personal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://toolupcom-my.sharepoint.com/personal/solomon_manamel_pcstools_com/Documents/Desktop/P/Planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="599" documentId="13_ncr:1_{AB593B95-CA86-472D-9472-78DA2E2AD5AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F3AE5DC-C7FC-4DF6-A19E-C4899706A2F2}"/>
+  <xr:revisionPtr revIDLastSave="602" documentId="13_ncr:1_{AB593B95-CA86-472D-9472-78DA2E2AD5AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F637B48-A5A8-42D5-8C38-AAA971BF7C61}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="1770" windowWidth="29040" windowHeight="15720" xr2:uid="{0AD46AC5-6205-4944-BA9B-94CEDC03FC4D}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="203">
   <si>
     <t>Be able to do a handstand</t>
   </si>
@@ -677,6 +677,9 @@
   <si>
     <t>Steam Deck</t>
   </si>
+  <si>
+    <t>Done</t>
+  </si>
 </sst>
 </file>
 
@@ -963,9 +966,6 @@
       </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -985,6 +985,9 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -1018,7 +1021,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1BD04884-7BD2-4EC0-8601-630D34CD5844}" name="Goals" displayName="Goals" ref="C8:J51" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1BD04884-7BD2-4EC0-8601-630D34CD5844}" name="Goals" displayName="Goals" ref="C8:J51" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="C8:J51" xr:uid="{1BD04884-7BD2-4EC0-8601-630D34CD5844}">
     <filterColumn colId="2">
       <filters>
@@ -1044,10 +1047,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2F67A716-A476-4F97-A4BE-083BC55A57BC}" name="wishlist" displayName="wishlist" ref="B2:C18" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2F67A716-A476-4F97-A4BE-083BC55A57BC}" name="wishlist" displayName="wishlist" ref="B2:C18" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="B2:C18" xr:uid="{2F67A716-A476-4F97-A4BE-083BC55A57BC}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{6857037D-85CE-4B6D-89D5-32E6C539BE03}" name="Wishlist" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{6857037D-85CE-4B6D-89D5-32E6C539BE03}" name="Wishlist" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{AF2F47ED-9D25-4B5B-86D0-F9374CE88BB6}" name="$"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1374,7 +1377,7 @@
   <dimension ref="A1:O73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E25" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1825,6 +1828,9 @@
       </c>
       <c r="E31" t="s">
         <v>155</v>
+      </c>
+      <c r="F31" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -3039,7 +3045,7 @@
       </c>
       <c r="C6" s="4">
         <f ca="1">MATCH(TODAY(),G:G)</f>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="U6" t="str" cm="1">
         <f t="array" ref="U6:BK7">TRANSPOSE(_xlfn.SORTBY(Goals[[Category]:[Sub Category]],Goals[Category]))</f>
@@ -3309,11 +3315,11 @@
     <row r="9" spans="2:76" x14ac:dyDescent="0.25">
       <c r="I9" s="22">
         <f ca="1">COUNTIF(I11:INDIRECT(_xlfn.CONCAT(CHAR(COLUMN()+64),today_index)),TRUE)/(TODAY()-$G$11)</f>
-        <v>0.14285714285714285</v>
+        <v>0.1</v>
       </c>
       <c r="J9" s="22">
         <f ca="1">COUNTIF(J11:INDIRECT(_xlfn.CONCAT(CHAR(COLUMN()+64),today_index)),TRUE)/(TODAY()-$G$11)</f>
-        <v>0.14285714285714285</v>
+        <v>0.1</v>
       </c>
       <c r="K9" s="22">
         <f ca="1">COUNTIF(K11:INDIRECT(_xlfn.CONCAT(CHAR(COLUMN()+64),today_index)),TRUE)/(TODAY()-$G$11)</f>
@@ -3325,7 +3331,7 @@
       </c>
       <c r="M9" s="22">
         <f ca="1">COUNTIF(M11:INDIRECT(_xlfn.CONCAT(CHAR(COLUMN()+64),today_index)),TRUE)/(TODAY()-$G$11)</f>
-        <v>0.14285714285714285</v>
+        <v>0.1</v>
       </c>
       <c r="N9" s="22">
         <f ca="1">COUNTIF(N11:INDIRECT(_xlfn.CONCAT(CHAR(COLUMN()+64),today_index)),TRUE)/(TODAY()-$G$11)</f>
@@ -20265,17 +20271,17 @@
   </sheetData>
   <autoFilter ref="E10:P10" xr:uid="{68DA2AD1-B9FC-471D-A935-E7E28162797C}"/>
   <mergeCells count="11">
-    <mergeCell ref="E74:E80"/>
-    <mergeCell ref="E81:E87"/>
-    <mergeCell ref="E53:E59"/>
-    <mergeCell ref="E60:E66"/>
-    <mergeCell ref="E67:E73"/>
     <mergeCell ref="E46:E52"/>
     <mergeCell ref="E11:E17"/>
     <mergeCell ref="E18:E24"/>
     <mergeCell ref="E25:E31"/>
     <mergeCell ref="E32:E38"/>
     <mergeCell ref="E39:E45"/>
+    <mergeCell ref="E74:E80"/>
+    <mergeCell ref="E81:E87"/>
+    <mergeCell ref="E53:E59"/>
+    <mergeCell ref="E60:E66"/>
+    <mergeCell ref="E67:E73"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="A10:XFD10">

</xml_diff>